<commit_message>
Correction remarque Et–Étage sur Windows
</commit_message>
<xml_diff>
--- a/kit/Resultats-EPUB3/Resultats-epub3.xlsx
+++ b/kit/Resultats-EPUB3/Resultats-epub3.xlsx
@@ -170,7 +170,7 @@
   </si>
   <si>
     <t>Narrateur stock
-Et prononce étage en début de ligne</t>
+Et prononcé étage si suivi d’un chiffre</t>
   </si>
   <si>
     <t>fulltitle</t>
@@ -1226,7 +1226,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>